<commit_message>
adding season finale correct answers
</commit_message>
<xml_diff>
--- a/resources/correct_answers.xlsx
+++ b/resources/correct_answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annes/Documents/Personal/GoT/GameOfThronesLeaguePythonOO/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64DBBE4-AAA6-6147-98DC-E15F76BC47B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A603009-8E83-0642-A75F-E50038551AD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
   <si>
     <t>simple_text</t>
   </si>
@@ -331,9 +331,6 @@
     <t>Dies</t>
   </si>
   <si>
-    <t>Arya kills the Knight's King</t>
-  </si>
-  <si>
     <t>The Hound kills Ser Gregor, Ser Gregor kills Qyburn</t>
   </si>
   <si>
@@ -356,13 +353,31 @@
   </si>
   <si>
     <t>question_number</t>
+  </si>
+  <si>
+    <t>No One/There will be no Iron Throne</t>
+  </si>
+  <si>
+    <t>Arya kills the Night's King</t>
+  </si>
+  <si>
+    <t>There is no prince that was promised</t>
+  </si>
+  <si>
+    <t>Edmure Tully, Robin Arryn</t>
+  </si>
+  <si>
+    <t>Nymeria, Ghost, Drogon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gilly and Samwell </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -493,6 +508,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -839,8 +861,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1198,15 +1221,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1218,7 +1241,7 @@
         <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1234,7 +1257,7 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1251,8 +1274,8 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>101</v>
+      <c r="E3" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1268,7 +1291,7 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1285,7 +1308,7 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1302,7 +1325,7 @@
       <c r="D6" t="b">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1319,7 +1342,7 @@
       <c r="D7" t="b">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1336,7 +1359,7 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1353,7 +1376,7 @@
       <c r="D9" t="b">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1370,7 +1393,7 @@
       <c r="D10" t="b">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1387,7 +1410,7 @@
       <c r="D11" t="b">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1404,7 +1427,7 @@
       <c r="D12" t="b">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1421,7 +1444,7 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1438,7 +1461,7 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1455,7 +1478,7 @@
       <c r="D15" t="b">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1472,7 +1495,7 @@
       <c r="D16" t="b">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1489,7 +1512,7 @@
       <c r="D17" t="b">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1506,7 +1529,7 @@
       <c r="D18" t="b">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1523,7 +1546,7 @@
       <c r="D19" t="b">
         <v>1</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1540,7 +1563,7 @@
       <c r="D20" t="b">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1557,7 +1580,7 @@
       <c r="D21" t="b">
         <v>1</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1574,7 +1597,7 @@
       <c r="D22" t="b">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1591,7 +1614,7 @@
       <c r="D23" t="b">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1608,7 +1631,7 @@
       <c r="D24" t="b">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1623,7 +1646,10 @@
         <v>6</v>
       </c>
       <c r="D25" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1637,7 +1663,10 @@
         <v>4</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1653,8 +1682,8 @@
       <c r="D27" t="b">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
-        <v>103</v>
+      <c r="E27" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1671,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1685,7 +1714,10 @@
         <v>4</v>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1719,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1736,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1753,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1770,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1784,7 +1816,10 @@
         <v>1</v>
       </c>
       <c r="D35" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1801,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1818,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1832,7 +1867,10 @@
         <v>1</v>
       </c>
       <c r="D38" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1846,7 +1884,10 @@
         <v>1</v>
       </c>
       <c r="D39" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1863,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1877,7 +1918,10 @@
         <v>1</v>
       </c>
       <c r="D41" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1891,7 +1935,10 @@
         <v>2</v>
       </c>
       <c r="D42" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1908,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1922,7 +1969,10 @@
         <v>2</v>
       </c>
       <c r="D44" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1939,7 +1989,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1956,7 +2006,7 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1970,7 +2020,10 @@
         <v>2</v>
       </c>
       <c r="D47" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1984,10 +2037,13 @@
         <v>4</v>
       </c>
       <c r="D48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -1998,10 +2054,13 @@
         <v>3</v>
       </c>
       <c r="D49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2013,6 +2072,9 @@
       </c>
       <c r="D50" t="b">
         <v>0</v>
+      </c>
+      <c r="E50">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>